<commit_message>
Running tests on the precision of maxcov
</commit_message>
<xml_diff>
--- a/Notes/Misc/MAXCOV_methods_precision.xlsx
+++ b/Notes/Misc/MAXCOV_methods_precision.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28340" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28340" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>corrent_pct</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>CONVEX HULL FROM DELAUNAY TRIANGLES</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>The most unprecise identification happens when the optimal triangle has a small inradius</t>
   </si>
 </sst>
 </file>
@@ -435,11 +441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2112016568"/>
-        <c:axId val="-2086794136"/>
+        <c:axId val="-2097980024"/>
+        <c:axId val="-2097916392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2112016568"/>
+        <c:axId val="-2097980024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +455,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086794136"/>
+        <c:crossAx val="-2097916392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086794136"/>
+        <c:axId val="-2097916392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -469,7 +475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112016568"/>
+        <c:crossAx val="-2097980024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -753,11 +759,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109699992"/>
-        <c:axId val="-2100597896"/>
+        <c:axId val="-2098994712"/>
+        <c:axId val="-2106828728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109699992"/>
+        <c:axId val="-2098994712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100597896"/>
+        <c:crossAx val="-2106828728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -775,7 +781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2100597896"/>
+        <c:axId val="-2106828728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109699992"/>
+        <c:crossAx val="-2098994712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1070,11 +1076,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2099940984"/>
-        <c:axId val="-2100037176"/>
+        <c:axId val="-2098717448"/>
+        <c:axId val="-2098522632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2099940984"/>
+        <c:axId val="-2098717448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100037176"/>
+        <c:crossAx val="-2098522632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1092,7 +1098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2100037176"/>
+        <c:axId val="-2098522632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1109,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099940984"/>
+        <c:crossAx val="-2098717448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1544,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1885,6 +1891,14 @@
       </c>
       <c r="G20" s="2">
         <v>0.58328999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2174,7 +2188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>

</xml_diff>